<commit_message>
Added the clubds class and made funtions to : 1. register students to clubs 2. view club details 3. add students to clubs
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -5,12 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="courses" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="student_courses" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="clubs" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="student_clubs" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t xml:space="preserve">student_admission</t>
   </si>
@@ -94,6 +96,27 @@
   </si>
   <si>
     <t xml:space="preserve">No. of Students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_clubs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_students_club</t>
   </si>
 </sst>
 </file>
@@ -168,13 +191,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -200,14 +227,14 @@
       <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -271,7 +298,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
@@ -329,18 +356,18 @@
   </sheetPr>
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="0" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="0" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.01"/>
   </cols>
   <sheetData>
@@ -395,4 +422,114 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="H3" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added the add course button to the GUI and it works
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -460,10 +460,10 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100">
-      <selection activeCell="H10" activeCellId="0" pane="topLeft" sqref="H10"/>
+      <selection activeCell="H8" activeCellId="0" pane="topLeft" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.2109375" defaultRowHeight="12.75" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.2265625" defaultRowHeight="12.75" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="3" width="16.14"/>
     <col customWidth="1" max="5" min="5" style="3" width="14.28"/>
@@ -518,42 +518,42 @@
     <row customHeight="1" ht="12.75" r="2" s="4">
       <c r="A2" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>Hasith</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>Dewmina</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>01/18/2006</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>M</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>Lesli Kumara</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>3456789</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>Ruwi, Muscat, Oman</t>
         </is>
       </c>
       <c r="J2" s="3" t="inlineStr">
@@ -597,7 +597,7 @@
       <selection activeCell="F4" activeCellId="0" pane="topLeft" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.75" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.75" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="3" width="9.289999999999999"/>
     <col customWidth="1" max="2" min="2" style="3" width="12.42"/>
@@ -676,7 +676,7 @@
       <selection activeCell="J2" activeCellId="0" pane="topLeft" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.75" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.75" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="3" width="9.710000000000001"/>
     <col customWidth="1" max="2" min="2" style="3" width="6.28"/>
@@ -779,7 +779,7 @@
       <selection activeCell="F4" activeCellId="0" pane="topLeft" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.75" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.75" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData>
     <row customHeight="1" ht="12.75" r="1" s="4">
       <c r="A1" s="3" t="inlineStr">
@@ -842,7 +842,7 @@
       <selection activeCell="H4" activeCellId="0" pane="topLeft" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.75" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.75" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="8" min="8" style="3" width="17.59"/>
   </cols>

</xml_diff>

<commit_message>
Expanded the back button in the student category
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -420,13 +420,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.28515625" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.28515625" defaultRowHeight="12.75"/>
   <cols>
     <col width="16.85546875" customWidth="1" style="1" min="1" max="1"/>
     <col width="14.28515625" customWidth="1" style="1" min="5" max="5"/>
@@ -479,44 +479,6 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1" s="1">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Hasith</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Dewmina</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>18/01/2006</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Lesli Kumara, Gangani Madawala</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>84593475893075894375Turi</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Ruwi, Muscat, Oman</t>
-        </is>
-      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>no. of Students</t>
@@ -525,7 +487,7 @@
     </row>
     <row r="3" ht="12.75" customHeight="1" s="1">
       <c r="J3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="1"/>
@@ -557,7 +519,7 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
     <col width="16.7109375" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="10.140625" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
@@ -613,6 +575,44 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Hasith</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Dewmina</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>18/01/2006</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Lesli Kumara, Gangani Madawala</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>84593475893075894375Turi</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Ruwi, Muscat, Oman</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>Num Students</t>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -679,7 +679,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="9.28515625" customWidth="1" style="1" min="1" max="1"/>
     <col width="12.42578125" customWidth="1" style="1" min="2" max="2"/>
@@ -757,7 +757,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="9.7109375" customWidth="1" style="1" min="1" max="1"/>
     <col width="6.28515625" customWidth="1" style="1" min="2" max="2"/>
@@ -921,7 +921,7 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="17.5703125" customWidth="1" style="1" min="8" max="8"/>
   </cols>

</xml_diff>

<commit_message>
Add some buttons to teacher and students
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15885" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="15885" windowWidth="28800" xWindow="390" yWindow="390"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" state="visible" r:id="rId1"/>
@@ -47,19 +47,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -420,23 +420,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="156" zoomScaleNormal="156">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.28515625" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
-    <col width="16.85546875" customWidth="1" style="1" min="1" max="1"/>
-    <col width="14.28515625" customWidth="1" style="1" min="5" max="5"/>
-    <col width="24.42578125" customWidth="1" style="1" min="6" max="6"/>
-    <col width="19.28515625" customWidth="1" style="1" min="7" max="7"/>
-    <col width="23.140625" customWidth="1" style="1" min="8" max="8"/>
-    <col width="13.85546875" bestFit="1" customWidth="1" style="1" min="10" max="10"/>
+    <col customWidth="1" max="1" min="1" style="1" width="16.85546875"/>
+    <col customWidth="1" max="5" min="5" style="1" width="14.28515625"/>
+    <col customWidth="1" max="6" min="6" style="1" width="24.42578125"/>
+    <col customWidth="1" max="7" min="7" style="1" width="19.28515625"/>
+    <col customWidth="1" max="8" min="8" style="1" width="23.140625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="1" width="13.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="1" s="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>student_admission</t>
@@ -478,100 +478,24 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1" s="1">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Hasith</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Dewmina</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>18/06/2006</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Lesli Kumara, Gangani Madwala</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>483573489579</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Ruwi, Muscat, Oman</t>
-        </is>
-      </c>
+    <row customHeight="1" ht="12.75" r="2" s="1">
       <c r="J2" t="inlineStr">
         <is>
           <t>no. of Students</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="12.75" customHeight="1" s="1">
-      <c r="A3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>hj</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>j</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>hj</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>hj</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>fdfd</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>hj</t>
-        </is>
-      </c>
+    <row customHeight="1" ht="12.75" r="3" s="1">
       <c r="J3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1" s="1"/>
-    <row r="5" ht="12.75" customHeight="1" s="1"/>
-    <row r="6" ht="12.75" customHeight="1" s="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="4" s="1"/>
+    <row customHeight="1" ht="12.75" r="5" s="1"/>
+    <row customHeight="1" ht="12.75" r="6" s="1"/>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" useFirstPageNumber="1" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -591,21 +515,21 @@
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="160" zoomScaleNormal="160">
       <selection activeCell="I12" sqref="I12:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
-    <col width="16.7109375" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="10.140625" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
-    <col width="10" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
-    <col width="10.5703125" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
-    <col width="7" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
-    <col width="29.28515625" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
-    <col width="17.7109375" bestFit="1" customWidth="1" style="1" min="7" max="7"/>
-    <col width="18.7109375" bestFit="1" customWidth="1" style="1" min="8" max="8"/>
-    <col width="12.85546875" bestFit="1" customWidth="1" style="1" min="10" max="10"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="16.7109375"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="1" width="10.140625"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="1" width="10"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="1" width="10.5703125"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="1" width="7"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="1" width="29.28515625"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="1" width="17.7109375"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="1" width="18.7109375"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="1" width="12.85546875"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -651,6 +575,44 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>hj</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>hj</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>hj</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>fdfd</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>hj</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>Num Students</t>
@@ -697,11 +659,11 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -713,23 +675,23 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="156" zoomScaleNormal="156">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
-    <col width="9.28515625" customWidth="1" style="1" min="1" max="1"/>
-    <col width="12.42578125" customWidth="1" style="1" min="2" max="2"/>
-    <col width="14.5703125" customWidth="1" style="1" min="3" max="3"/>
-    <col width="12" customWidth="1" style="1" min="4" max="4"/>
-    <col width="11.140625" customWidth="1" style="1" min="5" max="5"/>
-    <col width="29.5703125" customWidth="1" style="1" min="6" max="6"/>
-    <col width="8.5703125" customWidth="1" style="1" min="7" max="7"/>
-    <col width="18.7109375" customWidth="1" style="1" min="8" max="8"/>
+    <col customWidth="1" max="1" min="1" style="1" width="9.28515625"/>
+    <col customWidth="1" max="2" min="2" style="1" width="12.42578125"/>
+    <col customWidth="1" max="3" min="3" style="1" width="14.5703125"/>
+    <col customWidth="1" max="4" min="4" style="1" width="12"/>
+    <col customWidth="1" max="5" min="5" style="1" width="11.140625"/>
+    <col customWidth="1" max="6" min="6" style="1" width="29.5703125"/>
+    <col customWidth="1" max="7" min="7" style="1" width="8.5703125"/>
+    <col customWidth="1" max="8" min="8" style="1" width="18.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="1" s="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>course_id</t>
@@ -756,22 +718,22 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1" s="1"/>
-    <row r="3" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="2" s="1"/>
+    <row customHeight="1" ht="12.75" r="3" s="1">
       <c r="F3" t="inlineStr">
         <is>
           <t>No. of courses</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="4" s="1">
       <c r="F4" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -791,22 +753,22 @@
   </sheetPr>
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="156" zoomScaleNormal="156">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
-    <col width="9.7109375" customWidth="1" style="1" min="1" max="1"/>
-    <col width="6.28515625" customWidth="1" style="1" min="2" max="2"/>
-    <col width="9" customWidth="1" style="1" min="3" max="3"/>
-    <col width="9.28515625" customWidth="1" style="1" min="4" max="4"/>
-    <col width="12.42578125" customWidth="1" style="1" min="5" max="5"/>
-    <col width="8.42578125" customWidth="1" style="1" min="6" max="10"/>
-    <col width="14" customWidth="1" style="1" min="12" max="12"/>
+    <col customWidth="1" max="1" min="1" style="1" width="9.7109375"/>
+    <col customWidth="1" max="2" min="2" style="1" width="6.28515625"/>
+    <col customWidth="1" max="3" min="3" style="1" width="9"/>
+    <col customWidth="1" max="4" min="4" style="1" width="9.28515625"/>
+    <col customWidth="1" max="5" min="5" style="1" width="12.42578125"/>
+    <col customWidth="1" max="10" min="6" style="1" width="8.42578125"/>
+    <col customWidth="1" max="12" min="12" style="1" width="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="1" s="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>student_id</t>
@@ -858,22 +820,22 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1" s="1"/>
-    <row r="3" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="2" s="1"/>
+    <row customHeight="1" ht="12.75" r="3" s="1">
       <c r="L3" t="inlineStr">
         <is>
           <t>No. of Students</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="4" s="1">
       <c r="L4" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -893,13 +855,13 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="156" zoomScaleNormal="156">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="1" s="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>Club_ID</t>
@@ -921,21 +883,21 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="3" s="1">
       <c r="F3" t="inlineStr">
         <is>
           <t>num_clubs</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="4" s="1">
       <c r="F4" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -955,16 +917,16 @@
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="156" zoomScaleNormal="156">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
-    <col width="17.5703125" customWidth="1" style="1" min="8" max="8"/>
+    <col customWidth="1" max="8" min="8" style="1" width="17.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="1" s="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>Student_ID</t>
@@ -991,23 +953,23 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1" s="1"/>
-    <row r="3" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="2" s="1"/>
+    <row customHeight="1" ht="12.75" r="3" s="1">
       <c r="H3" t="inlineStr">
         <is>
           <t>num_students_club</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="12.75" customHeight="1" s="1">
+    <row customHeight="1" ht="12.75" r="4" s="1">
       <c r="H4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="5" ht="12.75" customHeight="1" s="1"/>
+    <row customHeight="1" ht="12.75" r="5" s="1"/>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Completed the Add course button for Admin
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="15885" windowWidth="28800" xWindow="390" yWindow="390"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,18 +15,33 @@
     <sheet name="student_clubs" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
       <family val="2"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -46,20 +62,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -416,87 +454,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="156" zoomScaleNormal="156">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.28515625" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.31640625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="16.85546875"/>
-    <col customWidth="1" max="5" min="5" style="1" width="14.28515625"/>
-    <col customWidth="1" max="6" min="6" style="1" width="24.42578125"/>
-    <col customWidth="1" max="7" min="7" style="1" width="19.28515625"/>
-    <col customWidth="1" max="8" min="8" style="1" width="23.140625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="1" width="13.85546875"/>
+    <col width="16.87" customWidth="1" style="3" min="1" max="1"/>
+    <col width="14.28" customWidth="1" style="3" min="5" max="5"/>
+    <col width="24.41" customWidth="1" style="3" min="6" max="6"/>
+    <col width="19.3" customWidth="1" style="3" min="7" max="7"/>
+    <col width="23.15" customWidth="1" style="3" min="8" max="8"/>
+    <col width="13.86" customWidth="1" style="3" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="12.75" r="1" s="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="12.75" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>student_admission</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>First Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Last Name</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>DoB</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Gender</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Guardian Names</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Guardian Telephone</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="2" s="1">
-      <c r="J2" t="inlineStr">
+    <row r="2" ht="12.75" customHeight="1" s="4">
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>no. of Students</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="3" s="1">
-      <c r="J3" t="n">
+    <row r="3" ht="12.75" customHeight="1" s="4">
+      <c r="J3" s="3" t="n">
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="4" s="1"/>
-    <row customHeight="1" ht="12.75" r="5" s="1"/>
-    <row customHeight="1" ht="12.75" r="6" s="1"/>
+    <row r="4" ht="12.75" customHeight="1" s="4"/>
+    <row r="5" ht="12.75" customHeight="1" s="4"/>
+    <row r="6" ht="12.75" customHeight="1" s="4"/>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" useFirstPageNumber="1" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>
@@ -509,232 +548,259 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="160" zoomScaleNormal="160">
-      <selection activeCell="I12" sqref="I12:I13"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="16.7109375"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="1" width="10.140625"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="1" width="10"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="1" width="10.5703125"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="1" width="7"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="1" width="29.28515625"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="1" width="17.7109375"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="1" width="18.7109375"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="1" width="12.85546875"/>
+    <col width="16.71" customWidth="1" style="3" min="1" max="1"/>
+    <col width="10.13" customWidth="1" style="3" min="2" max="2"/>
+    <col width="10" customWidth="1" style="3" min="3" max="3"/>
+    <col width="10.58" customWidth="1" style="3" min="4" max="4"/>
+    <col width="7" customWidth="1" style="3" min="5" max="5"/>
+    <col width="29.29" customWidth="1" style="3" min="6" max="6"/>
+    <col width="17.71" customWidth="1" style="3" min="7" max="7"/>
+    <col width="18.71" customWidth="1" style="3" min="8" max="8"/>
+    <col width="12.86" customWidth="1" style="3" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="12.75" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>student_admission</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>First Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Last Name</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>DoB</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Gender</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Guardian Names</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Guardian Telephone</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" ht="12.75" customHeight="1" s="4">
+      <c r="A2" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>hj</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>j</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>hj</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>hj</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>fdfd</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="3" t="inlineStr">
         <is>
           <t>hj</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>Num Students</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" ht="12.75" customHeight="1" s="4">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Dave</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Lee</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>02/01/2005</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>Sam Lee, Agnetha Lee</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>78t7r8te9ter</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="3" t="inlineStr">
         <is>
           <t>Ruwi, Muscat, Oman</t>
         </is>
       </c>
-      <c r="J3" t="n">
+      <c r="J3" s="3" t="n">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="156" zoomScaleNormal="156">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="9.28515625"/>
-    <col customWidth="1" max="2" min="2" style="1" width="12.42578125"/>
-    <col customWidth="1" max="3" min="3" style="1" width="14.5703125"/>
-    <col customWidth="1" max="4" min="4" style="1" width="12"/>
-    <col customWidth="1" max="5" min="5" style="1" width="11.140625"/>
-    <col customWidth="1" max="6" min="6" style="1" width="29.5703125"/>
-    <col customWidth="1" max="7" min="7" style="1" width="8.5703125"/>
-    <col customWidth="1" max="8" min="8" style="1" width="18.7109375"/>
+    <col width="9.289999999999999" customWidth="1" style="3" min="1" max="1"/>
+    <col width="12.42" customWidth="1" style="3" min="2" max="2"/>
+    <col width="14.57" customWidth="1" style="3" min="3" max="3"/>
+    <col width="11.99" customWidth="1" style="3" min="4" max="4"/>
+    <col width="11.14" customWidth="1" style="3" min="5" max="5"/>
+    <col width="29.57" customWidth="1" style="3" min="6" max="6"/>
+    <col width="8.57" customWidth="1" style="3" min="7" max="7"/>
+    <col width="18.71" customWidth="1" style="3" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="12.75" r="1" s="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="12.75" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>course_id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>course_name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>course_duration</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>prerequisites</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>instructors</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="2" s="1"/>
-    <row customHeight="1" ht="12.75" r="3" s="1">
-      <c r="F3" t="inlineStr">
+    <row r="2" ht="12.75" customHeight="1" s="4">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Maths</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>5 Days</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Basic Algebra</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Sam Davis</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1" s="4">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>No. of courses</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="4" s="1">
-      <c r="F4" t="n">
-        <v>0</v>
+    <row r="4" ht="12.75" customHeight="1" s="4">
+      <c r="F4" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>
@@ -747,96 +813,97 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="156" zoomScaleNormal="156">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="9.7109375"/>
-    <col customWidth="1" max="2" min="2" style="1" width="6.28515625"/>
-    <col customWidth="1" max="3" min="3" style="1" width="9"/>
-    <col customWidth="1" max="4" min="4" style="1" width="9.28515625"/>
-    <col customWidth="1" max="5" min="5" style="1" width="12.42578125"/>
-    <col customWidth="1" max="10" min="6" style="1" width="8.42578125"/>
-    <col customWidth="1" max="12" min="12" style="1" width="14"/>
+    <col width="9.710000000000001" customWidth="1" style="3" min="1" max="1"/>
+    <col width="6.28" customWidth="1" style="3" min="2" max="2"/>
+    <col width="9" customWidth="1" style="3" min="3" max="3"/>
+    <col width="9.289999999999999" customWidth="1" style="3" min="4" max="4"/>
+    <col width="12.42" customWidth="1" style="3" min="5" max="5"/>
+    <col width="8.41" customWidth="1" style="3" min="6" max="10"/>
+    <col width="14.01" customWidth="1" style="3" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="12.75" r="1" s="1">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="12.75" customHeight="1" s="4">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>student_id</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>fname</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>lname</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>course_id</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>course_name</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>g1</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>g2</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>g3</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>g4</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t>g5</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="2" s="1"/>
-    <row customHeight="1" ht="12.75" r="3" s="1">
-      <c r="L3" t="inlineStr">
+    <row r="2" ht="12.75" customHeight="1" s="4"/>
+    <row r="3" ht="12.75" customHeight="1" s="4">
+      <c r="L3" s="3" t="inlineStr">
         <is>
           <t>No. of Students</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="4" s="1">
-      <c r="L4" t="n">
+    <row r="4" ht="12.75" customHeight="1" s="4">
+      <c r="L4" s="3" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>
@@ -849,56 +916,57 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="156" zoomScaleNormal="156">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row customHeight="1" ht="12.75" r="1" s="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="12.75" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Club_ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Club_name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Subject</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="3" s="1">
-      <c r="F3" t="inlineStr">
+    <row r="3" ht="12.75" customHeight="1" s="4">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>num_clubs</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="4" s="1">
-      <c r="F4" t="n">
+    <row r="4" ht="12.75" customHeight="1" s="4">
+      <c r="F4" s="3" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>
@@ -911,66 +979,67 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="156" zoomScaleNormal="156">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col customWidth="1" max="8" min="8" style="1" width="17.5703125"/>
+    <col width="17.59" customWidth="1" style="3" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="12.75" r="1" s="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="12.75" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Student_ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>fname</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>lname</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Club_ID</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Club_name</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="2" s="1"/>
-    <row customHeight="1" ht="12.75" r="3" s="1">
-      <c r="H3" t="inlineStr">
+    <row r="2" ht="12.75" customHeight="1" s="4"/>
+    <row r="3" ht="12.75" customHeight="1" s="4">
+      <c r="H3" s="3" t="inlineStr">
         <is>
           <t>num_students_club</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="4" s="1">
-      <c r="H4" t="n">
+    <row r="4" ht="12.75" customHeight="1" s="4">
+      <c r="H4" s="3" t="n">
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="5" s="1"/>
+    <row r="5" ht="12.75" customHeight="1" s="4"/>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>

</xml_diff>

<commit_message>
Got the View student grades in a course working and started the remove student from courses
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t xml:space="preserve">student_admission</t>
   </si>
@@ -355,12 +355,12 @@
       <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.86"/>
   </cols>
@@ -453,13 +453,13 @@
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -499,10 +499,10 @@
       <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7"/>
@@ -618,7 +618,7 @@
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.42"/>
@@ -722,18 +722,18 @@
   </sheetPr>
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="1" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="1" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.01"/>
   </cols>
   <sheetData>
@@ -769,7 +769,38 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>56</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="L3" s="1" t="s">
         <v>58</v>
@@ -777,7 +808,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="L4" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -802,7 +833,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -850,7 +881,7 @@
       <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.59"/>
   </cols>
@@ -906,7 +937,7 @@
       <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10"/>

</xml_diff>

<commit_message>
Got the view course details function working and did some few UI tweaks
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Pycharm\University-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEE1965-6F7A-42C2-BBA1-5CCB1D46F53B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738FE676-802E-4FD1-AEC1-60ACCFD282EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14865" yWindow="1110" windowWidth="28800" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1135,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added a gimic to call the student's name when they login
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Pycharm\University-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738FE676-802E-4FD1-AEC1-60ACCFD282EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C464E2C-FD66-430E-AA81-A7AC14F8B055}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17325" yWindow="5295" windowWidth="28800" windowHeight="16335" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -1136,7 +1136,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1179,45 +1179,31 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
+      <c r="A4"/>
     </row>
     <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
+      <c r="A5"/>
       <c r="G5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
+      <c r="A6"/>
       <c r="G6">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
+      <c r="A7"/>
     </row>
     <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
+      <c r="A8"/>
     </row>
     <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
+      <c r="A9"/>
     </row>
     <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
+      <c r="A10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Got some stuff working but had some trouble with finding a solution to the student_passwd_assigning thing in the student_functions.py file......CONTINUE FROM LINE 51 IN student_functions.py
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Pycharm\University-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C464E2C-FD66-430E-AA81-A7AC14F8B055}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0896B9AF-911D-486E-8F01-EE6B67B99213}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17325" yWindow="5295" windowWidth="28800" windowHeight="16335" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8595" yWindow="1575" windowWidth="28800" windowHeight="16335" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -26,104 +26,62 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+  <si>
+    <t xml:space="preserve">Index No. </t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>DoB</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Guardian Names</t>
+  </si>
+  <si>
+    <t>Guardian Telephone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Hasith</t>
+  </si>
+  <si>
+    <t>Dewmina</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Lesli Kumara, Gangani Madawala</t>
+  </si>
+  <si>
+    <t>Ruwi, Muscat, Oman</t>
+  </si>
+  <si>
+    <t>no. of Students</t>
+  </si>
   <si>
     <t>student_admission</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>DoB</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Guardian Names</t>
-  </si>
-  <si>
-    <t>Guardian Telephone</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Hasith</t>
-  </si>
-  <si>
-    <t>Dewmina</t>
-  </si>
-  <si>
-    <t>447583497</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Lesli Kumara, Gangani Madawala</t>
-  </si>
-  <si>
-    <t>5347583475893479</t>
-  </si>
-  <si>
-    <t>Ruwi, Muscat, Oman</t>
-  </si>
-  <si>
-    <t>no. of Students</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>Lee</t>
-  </si>
-  <si>
-    <t>47589</t>
-  </si>
-  <si>
-    <t>Sam Lee, Agnetha Lee</t>
-  </si>
-  <si>
-    <t>845734895739</t>
-  </si>
-  <si>
-    <t>Lucy</t>
-  </si>
-  <si>
-    <t>Hillfigure</t>
-  </si>
-  <si>
-    <t>43857348957</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>David Hillfigure, Pauly Hillfigure</t>
-  </si>
-  <si>
-    <t>48378957389</t>
-  </si>
-  <si>
-    <t>5743895739</t>
-  </si>
-  <si>
-    <t>75894375849375</t>
+    <t>76678687</t>
+  </si>
+  <si>
+    <t>874857498379</t>
   </si>
   <si>
     <t>Num Students</t>
   </si>
   <si>
-    <t>02/01/2005</t>
-  </si>
-  <si>
-    <t>78t7r8te9ter</t>
-  </si>
-  <si>
     <t>course_id</t>
   </si>
   <si>
@@ -230,18 +188,6 @@
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>hasith435</t>
-  </si>
-  <si>
-    <t>ranger445</t>
-  </si>
-  <si>
-    <t>Savin</t>
   </si>
   <si>
     <t>num rows</t>
@@ -602,12 +548,12 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" style="1" customWidth="1"/>
@@ -642,89 +588,26 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="A2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
+      <c r="A3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
       <c r="J3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-    </row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -742,7 +625,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -760,7 +643,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -786,60 +669,36 @@
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
       <c r="J3">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -870,19 +729,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -890,16 +749,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -907,19 +766,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -927,16 +786,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -973,51 +832,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-    </row>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1047,21 +895,21 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1094,25 +942,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1136,75 +984,48 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4"/>
-    </row>
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5"/>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6"/>
       <c r="G6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7"/>
-    </row>
-    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8"/>
-    </row>
-    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9"/>
-    </row>
-    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10"/>
-    </row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Debug why the password verifier is not checking credentials in real time
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9600" yWindow="2730" windowWidth="28800" windowHeight="16335" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1560" yWindow="1545" windowWidth="28770" windowHeight="15900" tabRatio="500" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" state="visible" r:id="rId1"/>
@@ -433,13 +433,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.42578125" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col width="9.42578125" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="14.28515625" customWidth="1" style="1" min="5" max="5"/>
@@ -502,32 +502,32 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dewmina</t>
+          <t>hj</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>75438957</t>
+          <t>hjk</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>hj</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Lesli Kumara, Gangani Madawala</t>
+          <t>kh</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>578439574839</t>
+          <t>jkhhj</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Ruwi, Muscat, Oman</t>
+          <t>hjkh</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -547,41 +547,278 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>fdfd</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>hg</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>hg</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>hjg</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>hgj</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" s="1">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>fj</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>hj</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>jkh</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>jk</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1" s="1">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Agnetha</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>hjk</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>jh</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>jkh</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>jk</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>hj</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1" s="1">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>Lee</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>4485987</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Tim Lee, Agnetha Lee</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>45845743858</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Ruwi, Muscat, Oman</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1" s="1"/>
-    <row r="5" ht="12.75" customHeight="1" s="1"/>
-    <row r="6" ht="12.75" customHeight="1" s="1"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dffd</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>hj</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>hj</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>kh</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>jk</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>hj</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Garry</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fgfgf</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>jh</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>jhj</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>kh</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>jk</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Kumara</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>hjkh</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>jkhjh</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>hjkhjkh</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>hjkhh</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>hjk</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>hjkhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>`2h</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>hjk</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>jklh</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>jk</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>hjk</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>lhjk</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -608,7 +845,7 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="16.7109375" customWidth="1" style="1" min="1" max="1"/>
     <col width="10.140625" customWidth="1" style="1" min="2" max="2"/>
@@ -731,7 +968,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="9.28515625" customWidth="1" style="1" min="1" max="1"/>
     <col width="12.42578125" customWidth="1" style="1" min="2" max="2"/>
@@ -879,7 +1116,7 @@
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="9.7109375" customWidth="1" style="1" min="1" max="1"/>
     <col width="6.28515625" customWidth="1" style="1" min="2" max="2"/>
@@ -1043,7 +1280,7 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="17.5703125" customWidth="1" style="1" min="8" max="8"/>
   </cols>
@@ -1109,13 +1346,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="12.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="10" customWidth="1" style="1" min="2" max="2"/>
@@ -1169,8 +1406,35 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="12.75" customHeight="1" s="1"/>
+    <row r="4" ht="12.75" customHeight="1" s="1">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>student3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+    </row>
     <row r="5" ht="12.75" customHeight="1" s="1">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>student4</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Agnetha</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
           <t>num rows</t>
@@ -1178,13 +1442,68 @@
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="1">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>student5</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Lee</t>
+        </is>
+      </c>
       <c r="G6" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" ht="12.75" customHeight="1" s="1"/>
-    <row r="8" ht="12.75" customHeight="1" s="1"/>
-    <row r="9" ht="12.75" customHeight="1" s="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1" s="1">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>student6</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Garry</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="1" s="1">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>student7</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Kumara</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="1" s="1">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>student8</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>`2h</t>
+        </is>
+      </c>
+    </row>
     <row r="10" ht="12.75" customHeight="1" s="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Found out why the read_password feature was not working in real0time and fixed it
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1560" yWindow="1545" windowWidth="28770" windowHeight="15900" tabRatio="500" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15885" tabRatio="500" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" state="visible" r:id="rId1"/>
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
@@ -502,32 +502,32 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>hj</t>
+          <t>fdfdf</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>hjk</t>
+          <t>j</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>hj</t>
+          <t>kj</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>kh</t>
+          <t>klj</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>jkhhj</t>
+          <t>kl</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>hjkh</t>
+          <t>jjkl</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -542,41 +542,41 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dave</t>
+          <t>Lee</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>fdfd</t>
+          <t>jkljk</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>jkl</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>hg</t>
+          <t>jkl</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>hg</t>
+          <t>jk</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>hjg</t>
+          <t>lj</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>hgj</t>
+          <t>kljkl</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="1">
@@ -585,22 +585,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sam</t>
+          <t>Dave</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>fj</t>
+          <t>hj</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>hj</t>
+          <t>h</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>jkh</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -615,7 +615,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>hjk</t>
         </is>
       </c>
     </row>
@@ -625,37 +625,37 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Agnetha</t>
+          <t>Dave</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>hjk</t>
+          <t>hj</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>hj</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>khjk</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>h</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>jh</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>jkh</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>jk</t>
-        </is>
-      </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>hj</t>
+          <t>jkhjk</t>
         </is>
       </c>
     </row>
@@ -665,37 +665,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dffd</t>
+          <t>hjh</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>jkh</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>jkh</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>jk</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>hj</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>hj</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>kh</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>jk</t>
-        </is>
-      </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>hj</t>
+          <t>hjk</t>
         </is>
       </c>
     </row>
@@ -705,117 +705,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Garry</t>
+          <t>Agnetha</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>fgfgf</t>
+          <t>j</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>k</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>jh</t>
+          <t>kl</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>jhj</t>
+          <t>kl</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>kh</t>
+          <t>jk</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>jk</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Kumara</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>hjkh</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>jkhjh</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>hjkhjkh</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>hjkhh</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>hjk</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>hjkhj</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>`2h</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>hjk</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>jklh</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>jk</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>hjk</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>lhjk</t>
+          <t>lj</t>
         </is>
       </c>
     </row>
@@ -1346,10 +1266,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -1402,7 +1322,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dave</t>
+          <t>Lee</t>
         </is>
       </c>
     </row>
@@ -1417,7 +1337,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sam</t>
+          <t>Dave</t>
         </is>
       </c>
     </row>
@@ -1432,7 +1352,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Agnetha</t>
+          <t>Dave</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1452,11 +1372,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="1">
@@ -1470,40 +1390,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Garry</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" ht="12.75" customHeight="1" s="1">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>student7</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Kumara</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="12.75" customHeight="1" s="1">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>student8</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>`2h</t>
-        </is>
-      </c>
-    </row>
+          <t>Agnetha</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="1" s="1"/>
+    <row r="9" ht="12.75" customHeight="1" s="1"/>
     <row r="10" ht="12.75" customHeight="1" s="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Some problems are there with the change password feature where it says the current password is incorrect when the password enterd is correct...need to fix that....in line 330
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15885" tabRatio="500" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4365" yWindow="2100" windowWidth="28800" windowHeight="15855" tabRatio="500" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" state="visible" r:id="rId1"/>
@@ -1269,7 +1269,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>student1</t>
+          <t>ranger445</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">

</xml_diff>

<commit_message>
did some permission work for students
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -439,7 +439,7 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.42578125" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="9.42578125" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="14.28515625" customWidth="1" style="1" min="5" max="5"/>
@@ -765,7 +765,7 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="16.7109375" customWidth="1" style="1" min="1" max="1"/>
     <col width="10.140625" customWidth="1" style="1" min="2" max="2"/>
@@ -888,7 +888,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="9.28515625" customWidth="1" style="1" min="1" max="1"/>
     <col width="12.42578125" customWidth="1" style="1" min="2" max="2"/>
@@ -1036,7 +1036,7 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="9.7109375" customWidth="1" style="1" min="1" max="1"/>
     <col width="6.28515625" customWidth="1" style="1" min="2" max="2"/>
@@ -1138,6 +1138,27 @@
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="1">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Hasith</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>fdfdf</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Maths</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>No. of Students</t>
@@ -1145,8 +1166,29 @@
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="1">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Lee</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>jkljk</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Science</t>
+        </is>
+      </c>
       <c r="L4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1237,7 +1279,7 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="17.5703125" customWidth="1" style="1" min="8" max="8"/>
   </cols>
@@ -1309,7 +1351,7 @@
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="12.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="10" customWidth="1" style="1" min="2" max="2"/>

</xml_diff>

<commit_message>
started the notifications feature, continue on line 280
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Pycharm\University-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5972AFC-D7FB-453D-8179-D385ECD15F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA801CF-D2A9-418E-A5D3-E8439C60C0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="3165" windowWidth="28800" windowHeight="15855" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4320" yWindow="4485" windowWidth="28800" windowHeight="15855" tabRatio="661" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
   <si>
     <t xml:space="preserve">Index No. </t>
   </si>
@@ -54,15 +54,36 @@
     <t>Address</t>
   </si>
   <si>
+    <t>Hasith</t>
+  </si>
+  <si>
+    <t>Dewmina</t>
+  </si>
+  <si>
+    <t>01/18/2006</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Lesli Kumara, Gangani Madawala</t>
+  </si>
+  <si>
+    <t>74895738957</t>
+  </si>
+  <si>
+    <t>Ruwi, Muscat, Oman</t>
+  </si>
+  <si>
+    <t>no. of Students</t>
+  </si>
+  <si>
+    <t>student_admission</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>no. of Students</t>
-  </si>
-  <si>
-    <t>student_admission</t>
-  </si>
-  <si>
     <t>Num Students</t>
   </si>
   <si>
@@ -102,9 +123,6 @@
     <t>Bio, Chem, Phy</t>
   </si>
   <si>
-    <t>Sam, Lucy</t>
-  </si>
-  <si>
     <t>No. of courses</t>
   </si>
   <si>
@@ -117,9 +135,6 @@
     <t>Esaay Writing, Language</t>
   </si>
   <si>
-    <t>David, Matt</t>
-  </si>
-  <si>
     <t>student_id</t>
   </si>
   <si>
@@ -144,12 +159,6 @@
     <t>g5</t>
   </si>
   <si>
-    <t>Hasith</t>
-  </si>
-  <si>
-    <t>fdfdf</t>
-  </si>
-  <si>
     <t>No. of Students</t>
   </si>
   <si>
@@ -180,70 +189,61 @@
     <t>password</t>
   </si>
   <si>
-    <t>student2</t>
-  </si>
-  <si>
-    <t>Lee</t>
-  </si>
-  <si>
-    <t>student3</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>student4</t>
+    <t>student1</t>
   </si>
   <si>
     <t>num rows</t>
   </si>
   <si>
-    <t>student5</t>
+    <t>Teacher ID</t>
+  </si>
+  <si>
+    <t>Qualifications</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>num teachers</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Sender</t>
+  </si>
+  <si>
+    <t>Receiver</t>
+  </si>
+  <si>
+    <t>Notification ID</t>
+  </si>
+  <si>
+    <t>num notifications</t>
   </si>
   <si>
     <t>Sam</t>
   </si>
   <si>
-    <t>student6</t>
-  </si>
-  <si>
-    <t>Agnetha</t>
-  </si>
-  <si>
-    <t>student1</t>
-  </si>
-  <si>
-    <t>Teacher ID</t>
-  </si>
-  <si>
-    <t>Qualifications</t>
-  </si>
-  <si>
-    <t>Experience</t>
-  </si>
-  <si>
-    <t>num teachers</t>
-  </si>
-  <si>
-    <t>Topic</t>
-  </si>
-  <si>
-    <t>Sender</t>
-  </si>
-  <si>
-    <t>Receiver</t>
+    <t>David</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -266,12 +266,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,18 +618,37 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
       <c r="J2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -668,7 +688,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -697,28 +717,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -734,10 +754,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -754,19 +774,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -774,16 +794,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -791,19 +811,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -811,20 +831,23 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -841,7 +864,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -857,34 +880,34 @@
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -892,21 +915,21 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -936,21 +959,21 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -983,25 +1006,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1025,7 +1048,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1037,10 +1060,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1051,95 +1074,27 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>53</v>
-      </c>
-    </row>
+    </row>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="G5" t="s">
         <v>54</v>
       </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" t="s">
-        <v>57</v>
-      </c>
       <c r="G6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-    </row>
+    </row>
+    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1152,14 +1107,14 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1168,37 +1123,20 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1212,30 +1150,48 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84707451-CDC9-4EC2-91EF-300059D0DEC6}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
problem in line 472 in student functions
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Pycharm\University-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA801CF-D2A9-418E-A5D3-E8439C60C0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5A3E5A-A246-4960-BD01-12995245F1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="4485" windowWidth="28800" windowHeight="15855" tabRatio="661" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="710" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,15 @@
     <sheet name="student_clubs" sheetId="6" r:id="rId6"/>
     <sheet name="student_pswd" sheetId="7" r:id="rId7"/>
     <sheet name="Teachers" sheetId="8" r:id="rId8"/>
-    <sheet name="notifications" sheetId="9" r:id="rId9"/>
+    <sheet name="teacher_psswd" sheetId="9" r:id="rId9"/>
+    <sheet name="notifications" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t xml:space="preserve">Index No. </t>
   </si>
@@ -123,6 +124,9 @@
     <t>Bio, Chem, Phy</t>
   </si>
   <si>
+    <t>Sam</t>
+  </si>
+  <si>
     <t>No. of courses</t>
   </si>
   <si>
@@ -135,6 +139,9 @@
     <t>Esaay Writing, Language</t>
   </si>
   <si>
+    <t>David</t>
+  </si>
+  <si>
     <t>student_id</t>
   </si>
   <si>
@@ -207,25 +214,28 @@
     <t>num teachers</t>
   </si>
   <si>
-    <t>Topic</t>
-  </si>
-  <si>
-    <t>Sender</t>
-  </si>
-  <si>
-    <t>Receiver</t>
-  </si>
-  <si>
-    <t>Notification ID</t>
+    <t>Notification id</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>sender</t>
+  </si>
+  <si>
+    <t>receiver</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Course Enrollment</t>
+  </si>
+  <si>
+    <t>Hasith would like to enroll in the Maths</t>
   </si>
   <si>
     <t>num notifications</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>David</t>
   </si>
 </sst>
 </file>
@@ -665,6 +675,71 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J3"/>
@@ -820,10 +895,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -831,16 +906,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -880,13 +955,13 @@
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>19</v>
@@ -895,19 +970,19 @@
         <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -929,12 +1004,12 @@
     </row>
     <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -959,21 +1034,21 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1006,25 +1081,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1048,7 +1123,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1060,10 +1135,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1074,7 +1149,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -1084,7 +1159,7 @@
     <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1106,15 +1181,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1123,15 +1198,15 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1151,46 +1226,41 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="F3" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
for some reason the notification is not appearing
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Pycharm\University-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5A3E5A-A246-4960-BD01-12995245F1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165CACBA-24B2-4F01-82FD-321EC8F34DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="710" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3945" yWindow="3060" windowWidth="28800" windowHeight="15855" tabRatio="710" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
   <si>
     <t xml:space="preserve">Index No. </t>
   </si>
@@ -79,124 +79,139 @@
     <t>no. of Students</t>
   </si>
   <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>hj</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>jhj</t>
+  </si>
+  <si>
     <t>student_admission</t>
   </si>
   <si>
+    <t>Num Students</t>
+  </si>
+  <si>
+    <t>course_id</t>
+  </si>
+  <si>
+    <t>course_name</t>
+  </si>
+  <si>
+    <t>course_duration</t>
+  </si>
+  <si>
+    <t>prerequisites</t>
+  </si>
+  <si>
+    <t>instructors</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>5 Days</t>
+  </si>
+  <si>
+    <t>Basic Algebra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sam </t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>4 Days</t>
+  </si>
+  <si>
+    <t>Bio, Chem, Phy</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>No. of courses</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>7 Days</t>
+  </si>
+  <si>
+    <t>Esaay Writing, Language</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>student_id</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>g2</t>
+  </si>
+  <si>
+    <t>g3</t>
+  </si>
+  <si>
+    <t>g4</t>
+  </si>
+  <si>
+    <t>g5</t>
+  </si>
+  <si>
+    <t>No. of Students</t>
+  </si>
+  <si>
+    <t>Club_ID</t>
+  </si>
+  <si>
+    <t>Club_name</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>num_clubs</t>
+  </si>
+  <si>
+    <t>Student_ID</t>
+  </si>
+  <si>
+    <t>num_students_club</t>
+  </si>
+  <si>
+    <t>index number</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>Num Students</t>
-  </si>
-  <si>
-    <t>course_id</t>
-  </si>
-  <si>
-    <t>course_name</t>
-  </si>
-  <si>
-    <t>course_duration</t>
-  </si>
-  <si>
-    <t>prerequisites</t>
-  </si>
-  <si>
-    <t>instructors</t>
-  </si>
-  <si>
-    <t>Maths</t>
-  </si>
-  <si>
-    <t>5 Days</t>
-  </si>
-  <si>
-    <t>Basic Algebra</t>
-  </si>
-  <si>
-    <t>Sam Davis</t>
-  </si>
-  <si>
-    <t>Science</t>
-  </si>
-  <si>
-    <t>4 Days</t>
-  </si>
-  <si>
-    <t>Bio, Chem, Phy</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>No. of courses</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>7 Days</t>
-  </si>
-  <si>
-    <t>Esaay Writing, Language</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>student_id</t>
-  </si>
-  <si>
-    <t>fname</t>
-  </si>
-  <si>
-    <t>lname</t>
-  </si>
-  <si>
-    <t>g1</t>
-  </si>
-  <si>
-    <t>g2</t>
-  </si>
-  <si>
-    <t>g3</t>
-  </si>
-  <si>
-    <t>g4</t>
-  </si>
-  <si>
-    <t>g5</t>
-  </si>
-  <si>
-    <t>No. of Students</t>
-  </si>
-  <si>
-    <t>Club_ID</t>
-  </si>
-  <si>
-    <t>Club_name</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>num_clubs</t>
-  </si>
-  <si>
-    <t>Student_ID</t>
-  </si>
-  <si>
-    <t>num_students_club</t>
-  </si>
-  <si>
-    <t>index number</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>student1</t>
+    <t>student2</t>
   </si>
   <si>
     <t>num rows</t>
@@ -211,9 +226,21 @@
     <t>Experience</t>
   </si>
   <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Maths Phd</t>
+  </si>
+  <si>
+    <t>5 Years</t>
+  </si>
+  <si>
     <t>num teachers</t>
   </si>
   <si>
+    <t>lecturer1</t>
+  </si>
+  <si>
     <t>Notification id</t>
   </si>
   <si>
@@ -229,7 +256,7 @@
     <t>description</t>
   </si>
   <si>
-    <t>Course Enrollment</t>
+    <t>COURSE ENROLLMENT</t>
   </si>
   <si>
     <t>Hasith would like to enroll in the Maths</t>
@@ -588,7 +615,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -657,8 +684,32 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -685,29 +736,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -715,19 +766,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -763,7 +814,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -788,37 +839,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +859,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E15" sqref="E14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -849,19 +876,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -869,16 +896,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -886,19 +913,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -906,16 +933,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -939,7 +966,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -955,34 +982,34 @@
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -999,17 +1026,17 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1027,28 +1054,28 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1081,25 +1108,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
         <v>51</v>
-      </c>
-      <c r="B1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1122,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1135,10 +1162,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1149,22 +1176,32 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1181,15 +1218,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1198,20 +1235,37 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1229,7 +1283,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1242,26 +1296,34 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
for some reason the login name does not equal the receiver name and the check_name_validity function in the student_functions.py file is not working.....it is at the very bottom of the file
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Pycharm\University-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165CACBA-24B2-4F01-82FD-321EC8F34DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E961D6-6893-4C16-8796-CCDA3D3762F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="3060" windowWidth="28800" windowHeight="15855" tabRatio="710" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="710" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
   <si>
     <t xml:space="preserve">Index No. </t>
   </si>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1030,13 +1030,43 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
       <c r="L3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
       <c r="L4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
got the notification system working.....have to make the system to notify the students when they get accepted to the course and when they get denied by the teacher.
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Pycharm\University-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E961D6-6893-4C16-8796-CCDA3D3762F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919DFF56-DBEA-4BA7-B7F1-FAF275891A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="710" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
   <si>
     <t xml:space="preserve">Index No. </t>
   </si>
@@ -124,7 +124,7 @@
     <t>Basic Algebra</t>
   </si>
   <si>
-    <t xml:space="preserve">Sam </t>
+    <t>Matt</t>
   </si>
   <si>
     <t>Science</t>
@@ -226,7 +226,7 @@
     <t>Experience</t>
   </si>
   <si>
-    <t>Davis</t>
+    <t>Peterson</t>
   </si>
   <si>
     <t>Maths Phd</t>
@@ -235,12 +235,24 @@
     <t>5 Years</t>
   </si>
   <si>
+    <t>Henchkins</t>
+  </si>
+  <si>
+    <t>jh</t>
+  </si>
+  <si>
     <t>num teachers</t>
   </si>
   <si>
     <t>lecturer1</t>
   </si>
   <si>
+    <t>lecturer2</t>
+  </si>
+  <si>
+    <t>Lucy</t>
+  </si>
+  <si>
     <t>Notification id</t>
   </si>
   <si>
@@ -254,12 +266,6 @@
   </si>
   <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>COURSE ENROLLMENT</t>
-  </si>
-  <si>
-    <t>Hasith would like to enroll in the Maths</t>
   </si>
   <si>
     <t>num notifications</t>
@@ -731,7 +737,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -746,44 +752,34 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -859,7 +855,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="E15" sqref="E14:E15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1013,60 +1009,25 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
     </row>
     <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
       <c r="L3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
       <c r="L4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1180,7 +1141,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1220,7 +1181,7 @@
         <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1249,7 +1210,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1276,7 +1237,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>65</v>
@@ -1289,13 +1250,28 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1340,20 +1316,29 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got the remove notifications function working ( have to make the cells shift one cell up )....the notificiation system does not work when 2 or more students send requests before the lecturer accepts one of them...continue from line 168 2mrw
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4155" yWindow="2460" windowWidth="28800" windowHeight="15885" tabRatio="710" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2970" yWindow="3870" windowWidth="28770" windowHeight="15885" tabRatio="710" firstSheet="0" activeTab="9" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" state="visible" r:id="rId1"/>
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -574,10 +574,49 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1" s="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" s="1">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Lucy</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Henckins</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>hjh</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>hjhj</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>hjhj</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>hjhjhj</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>hjh</t>
+        </is>
+      </c>
+    </row>
     <row r="5" ht="12.75" customHeight="1" s="1"/>
     <row r="6" ht="12.75" customHeight="1" s="1"/>
     <row r="7" ht="12.75" customHeight="1" s="1"/>
@@ -601,9 +640,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -657,15 +696,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>COURSE ENROLLMENT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Lucy</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Matt</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Lucy would like to enroll in the Maths</t>
+        </is>
+      </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
     </row>
+    <row r="4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -913,9 +971,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+    <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -984,16 +1042,16 @@
     </row>
     <row r="2" ht="12.75" customHeight="1" s="1">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dave</t>
+          <t>Hasith</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Dewmina</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -1006,6 +1064,27 @@
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="1">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Lucy</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Henckins</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Maths</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>No. of Students</t>
@@ -1013,10 +1092,84 @@
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="1">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Lucy</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Henckins</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Maths</t>
+        </is>
+      </c>
       <c r="L4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Lucy</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Henckins</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>1</v>
       </c>
-    </row>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Maths</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Lucy</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Henckins</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Maths</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup orientation="portrait" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
@@ -1231,7 +1384,21 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="12.75" customHeight="1" s="1"/>
+    <row r="4" ht="12.75" customHeight="1" s="1">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>student3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Lucy</t>
+        </is>
+      </c>
+    </row>
     <row r="5" ht="12.75" customHeight="1" s="1">
       <c r="G5" t="inlineStr">
         <is>
@@ -1241,7 +1408,7 @@
     </row>
     <row r="6" ht="12.75" customHeight="1" s="1">
       <c r="G6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="1"/>

</xml_diff>

<commit_message>
Got some where with the previous error. The program for some reason seems to run twice and returns the same value twice....need to fix this as this causes the same student to be registered to the same course twice eventhough they sent the request once
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2970" yWindow="3870" windowWidth="28770" windowHeight="15885" tabRatio="710" firstSheet="0" activeTab="9" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="8085" yWindow="3090" windowWidth="28770" windowHeight="15885" tabRatio="710" firstSheet="0" activeTab="9" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" state="visible" r:id="rId1"/>
@@ -431,13 +431,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.42578125" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col width="9.42578125" customWidth="1" style="1" min="1" max="1"/>
     <col width="14.28515625" customWidth="1" style="1" min="5" max="5"/>
@@ -505,27 +505,27 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>01/18/2006</t>
+          <t>hj</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>h</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Lesli Kumara, Gangani Madawala</t>
+          <t>jh</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>74895738957</t>
+          <t>j</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Ruwi, Muscat, Oman</t>
+          <t>hj</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -550,22 +550,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>hj</t>
+          <t>hjh</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>hj</t>
+          <t>jhj</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>hj</t>
+          <t>h</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>jh</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -574,49 +574,10 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1" s="1">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Lucy</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Henckins</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>hjh</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>hjhj</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>hjhj</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>hjhjhj</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>hjh</t>
-        </is>
-      </c>
-    </row>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" s="1"/>
     <row r="5" ht="12.75" customHeight="1" s="1"/>
     <row r="6" ht="12.75" customHeight="1" s="1"/>
     <row r="7" ht="12.75" customHeight="1" s="1"/>
@@ -640,13 +601,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
     <col width="12.140625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="22.5703125" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
@@ -684,11 +645,29 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>COURSE ENROLLMENT</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Hasith</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Matt</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Hasith would like to enroll in the Maths</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>num notifications</t>
@@ -696,34 +675,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>COURSE ENROLLMENT</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Lucy</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Matt</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Lucy would like to enroll in the Maths</t>
-        </is>
-      </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -741,7 +696,7 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="16.7109375" customWidth="1" style="1" min="1" max="1"/>
     <col width="10.140625" customWidth="1" style="1" min="2" max="2"/>
@@ -826,7 +781,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="9.28515625" customWidth="1" style="1" min="1" max="1"/>
     <col width="12.42578125" customWidth="1" style="1" min="2" max="2"/>
@@ -971,13 +926,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="9.7109375" customWidth="1" style="1" min="1" max="1"/>
     <col width="6.28515625" customWidth="1" style="1" min="2" max="2"/>
@@ -1065,16 +1020,16 @@
     </row>
     <row r="3" ht="12.75" customHeight="1" s="1">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Lucy</t>
+          <t>Hasith</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Henckins</t>
+          <t>Dewmina</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -1092,84 +1047,10 @@
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="1">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Lucy</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Henckins</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Maths</t>
-        </is>
-      </c>
       <c r="L4" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Lucy</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Henckins</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Maths</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Lucy</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Henckins</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Maths</t>
-        </is>
-      </c>
-    </row>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup orientation="portrait" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
@@ -1258,7 +1139,7 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="17.5703125" customWidth="1" style="1" min="8" max="8"/>
   </cols>
@@ -1330,7 +1211,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col width="12.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="10" customWidth="1" style="1" min="2" max="2"/>
@@ -1384,21 +1265,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="12.75" customHeight="1" s="1">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>student3</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Lucy</t>
-        </is>
-      </c>
-    </row>
+    <row r="4" ht="12.75" customHeight="1" s="1"/>
     <row r="5" ht="12.75" customHeight="1" s="1">
       <c r="G5" t="inlineStr">
         <is>
@@ -1408,7 +1275,7 @@
     </row>
     <row r="6" ht="12.75" customHeight="1" s="1">
       <c r="G6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="1"/>
@@ -1430,7 +1297,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1468,49 +1335,26 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Matt</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Peterson</t>
+          <t>j</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Maths Phd</t>
+          <t>kjk</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5 Years</t>
+          <t>j</t>
         </is>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="1">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Sam</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Henchkins</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>jh</t>
-        </is>
-      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>num teachers</t>
@@ -1519,7 +1363,7 @@
     </row>
     <row r="4" ht="12.75" customHeight="1" s="1">
       <c r="H4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1548,7 +1392,7 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
     <col width="12.140625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="8.85546875" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
@@ -1590,16 +1434,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>lecturer2</t>
+          <t>lecturer1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Lucy</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">

</xml_diff>

<commit_message>
got rid of the notification system code and started to work on the new more robust one
</commit_message>
<xml_diff>
--- a/university.xlsx
+++ b/university.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3225" yWindow="2775" windowWidth="28770" windowHeight="15885" tabRatio="710" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15885" tabRatio="710" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" state="visible" r:id="rId1"/>
@@ -437,7 +437,7 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.42578125" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="9.42578125" customWidth="1" style="1" min="1" max="1"/>
     <col width="14.28515625" customWidth="1" style="1" min="5" max="5"/>
@@ -601,13 +601,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="12.140625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="22.5703125" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
@@ -649,59 +649,10 @@
         </is>
       </c>
       <c r="H1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>COURSE ENROLLMENT</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Hasith</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Matt</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Hasith would like to enroll in the Maths</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>COURSE ENROLLMENT</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Hasith</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Matt</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Hasith would like to enroll in the Maths</t>
-        </is>
-      </c>
-    </row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -719,7 +670,7 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="16.7109375" customWidth="1" style="1" min="1" max="1"/>
     <col width="10.140625" customWidth="1" style="1" min="2" max="2"/>
@@ -804,7 +755,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="9.28515625" customWidth="1" style="1" min="1" max="1"/>
     <col width="12.42578125" customWidth="1" style="1" min="2" max="2"/>
@@ -952,10 +903,10 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="9.7109375" customWidth="1" style="1" min="1" max="1"/>
     <col width="6.28515625" customWidth="1" style="1" min="2" max="2"/>
@@ -1042,27 +993,6 @@
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="1">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Hasith</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Dewmina</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Maths</t>
-        </is>
-      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>No. of Students</t>
@@ -1071,7 +1001,7 @@
     </row>
     <row r="4" ht="12.75" customHeight="1" s="1">
       <c r="L4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1162,7 +1092,7 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="17.5703125" customWidth="1" style="1" min="8" max="8"/>
   </cols>
@@ -1234,7 +1164,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="12.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="10" customWidth="1" style="1" min="2" max="2"/>
@@ -1415,7 +1345,7 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="12.140625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="8.85546875" bestFit="1" customWidth="1" style="1" min="2" max="2"/>

</xml_diff>